<commit_message>
Done initiation of workpaper and  Import trial balance with new format
</commit_message>
<xml_diff>
--- a/public/uploads/xls/trialbalanceformat.xlsx
+++ b/public/uploads/xls/trialbalanceformat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Trial Balance" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,6 @@
     <t>Account Type</t>
   </si>
   <si>
-    <t>Debit - Year to date</t>
-  </si>
-  <si>
-    <t>Credit - Year to date</t>
-  </si>
-  <si>
     <t>Sale of Services</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>Retained Earnings</t>
+  </si>
+  <si>
+    <t>Year to date</t>
+  </si>
+  <si>
+    <t>Past Year</t>
   </si>
 </sst>
 </file>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -228,9 +228,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -555,7 +552,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -564,7 +561,7 @@
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -578,10 +575,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -589,271 +586,271 @@
         <v>210</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-7875215</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-7875215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>7875215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7">
+        <v>5415788</v>
+      </c>
+      <c r="E3" s="7">
+        <v>5415788</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8">
-        <v>5415788</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="7">
+        <v>338000</v>
+      </c>
+      <c r="E4" s="7">
+        <v>338000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8">
-        <v>338000</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7">
+        <v>33120</v>
+      </c>
+      <c r="E5" s="7">
+        <v>33120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8">
-        <v>33120</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7">
+        <v>20339</v>
+      </c>
+      <c r="E6" s="7">
+        <v>20339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="8">
-        <v>20339</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7">
+        <v>306921</v>
+      </c>
+      <c r="E7" s="7">
+        <v>306921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="8">
-        <v>306921</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="D8" s="7">
+        <v>3501263.87</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3501263.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8">
-        <v>3501263.87</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1735000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1735000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1735000</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7">
+        <v>553539</v>
+      </c>
+      <c r="E10" s="7">
+        <v>553539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="8">
-        <v>553539</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7">
+        <v>471000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="8">
-        <v>471000</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="D12" s="7">
+        <v>15238000</v>
+      </c>
+      <c r="E12" s="7">
+        <v>15238000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="8">
-        <v>15238000</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-235000</v>
+      </c>
+      <c r="E13" s="6">
+        <v>-235000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <v>235000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="D14" s="6">
+        <v>-3500</v>
+      </c>
+      <c r="E14" s="6">
+        <v>-3500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="D15" s="6">
+        <v>-5718554</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-5718554</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <v>5718554</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="D16" s="6">
+        <v>-13302057</v>
+      </c>
+      <c r="E16" s="6">
+        <v>-13302057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
-        <v>13302057</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
-        <v>478644.87</v>
+      <c r="C17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="6">
+        <v>-478644.87</v>
+      </c>
+      <c r="E17" s="6">
+        <v>-478644.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>